<commit_message>
Tabela Dinâmica - Filtro de Data
</commit_message>
<xml_diff>
--- a/Dinamicos__Tabela_e_Grfico.xlsx
+++ b/Dinamicos__Tabela_e_Grfico.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMAN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMAN\Desktop\Curso-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFBFB1D-4AD0-4B1B-85E0-0AA79C7EDDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3FA96E-CF47-494D-AD74-4F5EDC892AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="49">
   <si>
     <t>Nome</t>
   </si>
@@ -137,6 +137,45 @@
   </si>
   <si>
     <t>Soma de Quantidade Comprada</t>
+  </si>
+  <si>
+    <t>jan</t>
+  </si>
+  <si>
+    <t>fev</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>nov</t>
+  </si>
+  <si>
+    <t>dez</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>Trim1</t>
+  </si>
+  <si>
+    <t>Trim3</t>
+  </si>
+  <si>
+    <t>Trim4</t>
   </si>
 </sst>
 </file>
@@ -267,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -292,6 +331,15 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1072,8 +1120,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C41F5C1-33BF-4845-B126-616980157B86}" name="Tabela dinâmica1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="18">
-  <location ref="A3:B29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C41F5C1-33BF-4845-B126-616980157B86}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="18">
+  <location ref="A3:B36" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
       <items count="21">
@@ -1102,7 +1150,7 @@
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="6">
-        <item x="4"/>
+        <item sd="0" x="4"/>
         <item x="2"/>
         <item x="3"/>
         <item x="0"/>
@@ -1111,10 +1159,10 @@
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0">
+    <pivotField axis="axisRow" numFmtId="164" showAll="0">
       <items count="15">
         <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
+        <item x="1"/>
         <item sd="0" x="2"/>
         <item sd="0" x="3"/>
         <item sd="0" x="4"/>
@@ -1132,109 +1180,133 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
+        <item x="1"/>
         <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
+        <item x="3"/>
+        <item x="4"/>
         <item sd="0" x="5"/>
         <item t="default" sd="0"/>
       </items>
     </pivotField>
-    <pivotField showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="8">
         <item sd="0" x="0"/>
         <item sd="0" x="1"/>
         <item sd="0" x="2"/>
         <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
+        <item x="4"/>
+        <item x="5"/>
         <item sd="0" x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="2">
+  <rowFields count="5">
+    <field x="7"/>
+    <field x="6"/>
+    <field x="3"/>
     <field x="1"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="26">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
+  <rowItems count="33">
     <i>
       <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
     </i>
     <i>
       <x v="2"/>
     </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
     <i>
       <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
     </i>
     <i>
       <x v="4"/>
     </i>
     <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="4">
+      <x v="14"/>
+    </i>
+    <i r="3">
+      <x v="3"/>
+    </i>
+    <i r="4">
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="4">
+      <x v="3"/>
+    </i>
+    <i r="3">
+      <x v="2"/>
+    </i>
+    <i r="4">
+      <x v="1"/>
+    </i>
+    <i r="4">
+      <x v="10"/>
+    </i>
+    <i r="3">
+      <x v="3"/>
+    </i>
+    <i r="4">
+      <x v="9"/>
+    </i>
+    <i r="4">
+      <x v="19"/>
+    </i>
+    <i r="3">
+      <x v="4"/>
+    </i>
+    <i r="4">
       <x v="13"/>
     </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="18"/>
+    <i r="2">
+      <x v="2"/>
     </i>
     <i t="grand">
       <x/>
@@ -1246,17 +1318,6 @@
   <dataFields count="1">
     <dataField name="Soma de Quantidade Comprada" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="17" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -1532,7 +1593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457CE7E0-6BA7-4D60-89A1-FE9124C86CC7}">
-  <dimension ref="A3:B29"/>
+  <dimension ref="A3:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1540,7 +1601,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1555,209 +1616,265 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B4" s="19">
-        <v>13506</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>21</v>
+      <c r="A5" s="17" t="s">
+        <v>42</v>
       </c>
       <c r="B5" s="19">
-        <v>1670</v>
+        <v>476</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>16</v>
+      <c r="A6" s="17" t="s">
+        <v>43</v>
       </c>
       <c r="B6" s="19">
-        <v>5858</v>
+        <v>3813</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>11</v>
+      <c r="A7" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="B7" s="19">
-        <v>2166</v>
+        <v>50374</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="B8" s="19">
-        <v>3812</v>
+        <v>2850</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="19">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="19">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="19">
-        <v>11883</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="19">
-        <v>6258</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>9</v>
-      </c>
       <c r="B11" s="19">
-        <v>1374</v>
+        <v>987</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>14</v>
+      <c r="A12" s="22" t="s">
+        <v>19</v>
       </c>
       <c r="B12" s="19">
-        <v>3047</v>
+        <v>987</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>19</v>
+      <c r="A13" s="21" t="s">
+        <v>22</v>
       </c>
       <c r="B13" s="19">
-        <v>1204</v>
+        <v>987</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>25</v>
+      <c r="A14" s="22" t="s">
+        <v>2</v>
       </c>
       <c r="B14" s="19">
-        <v>20126</v>
+        <v>987</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>15</v>
+      <c r="A15" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="B15" s="19">
-        <v>5083</v>
+        <v>820</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B16" s="19">
-        <v>3578</v>
+        <v>16725</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>5</v>
+      <c r="A17" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="B17" s="19">
-        <v>9808</v>
+        <v>16725</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B18" s="19">
-        <v>1657</v>
+        <v>30799</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>22</v>
+      <c r="A19" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="B19" s="19">
-        <v>19524</v>
+        <v>20901</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>17</v>
+      <c r="A20" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="B20" s="19">
-        <v>9755</v>
+        <v>9898</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>2</v>
+      <c r="A21" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="B21" s="19">
-        <v>3904</v>
+        <v>21976</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B22" s="19">
-        <v>2129</v>
+        <v>21976</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="19">
+        <v>2181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="19">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="19">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="19">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="19">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="19">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="19">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="19">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="19">
-        <v>3736</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="B32" s="19">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="19">
-        <v>11784</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+      <c r="B33" s="19">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="19">
-        <v>1162</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="19">
-        <v>1071</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="19">
-        <v>5762</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="19">
-        <v>3789</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="B34" s="19">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="19">
+        <v>19795</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B36" s="19">
         <v>76823</v>
       </c>
     </row>

</xml_diff>